<commit_message>
- validasi penilaian (done) - perbaikan report penilaian (done)
</commit_message>
<xml_diff>
--- a/uploads/penilaian_strakom.xlsx
+++ b/uploads/penilaian_strakom.xlsx
@@ -201,32 +201,32 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Kabupaten Administrasi Kepulauan Seribu</t>
+          <t>Badan Kesatuan Bangsa Dan Politik</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>testingss</t>
+          <t>Pengembangan Smart City Melalui JAKI</t>
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>2.67</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>28.75</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>51.42</v>
+        <v>69</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>bagus</t>
         </is>
       </c>
     </row>

</xml_diff>